<commit_message>
Agrega 'Hola' en A1
</commit_message>
<xml_diff>
--- a/HojadeCalculo.xlsx
+++ b/HojadeCalculo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
@@ -11,8 +11,16 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Hola</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -60,7 +68,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Oficina">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -98,7 +106,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Oficina">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -168,7 +176,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Oficina">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -347,7 +355,13 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>

</xml_diff>